<commit_message>
Adding input data quality checks
</commit_message>
<xml_diff>
--- a/input_data.xlsx
+++ b/input_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11008"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chloe.hawker\Desktop\Data Engineer Hometask\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/george.adye/Documents/git/data_model_task/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{361BA793-1085-4553-993A-52ADA1A37F35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBDAFFCF-9259-474E-BEB8-6336E74A60F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="23260" windowHeight="12580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="in" sheetId="1" r:id="rId1"/>
@@ -1243,11 +1243,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1297,7 +1299,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -1347,7 +1349,7 @@
         <v>44276</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>28</v>
       </c>
@@ -1397,7 +1399,7 @@
         <v>44272</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>39</v>
       </c>
@@ -1447,7 +1449,7 @@
         <v>44272</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>43</v>
       </c>
@@ -1497,7 +1499,7 @@
         <v>44272</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>44</v>
       </c>
@@ -1547,7 +1549,7 @@
         <v>44272</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>47</v>
       </c>
@@ -1597,7 +1599,7 @@
         <v>44210</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>55</v>
       </c>
@@ -1647,7 +1649,7 @@
         <v>44210</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>56</v>
       </c>
@@ -1697,7 +1699,7 @@
         <v>44210</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>58</v>
       </c>
@@ -1747,7 +1749,7 @@
         <v>44210</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>60</v>
       </c>
@@ -1794,7 +1796,7 @@
         <v>44296</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>66</v>
       </c>
@@ -1844,7 +1846,7 @@
         <v>44223</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>74</v>
       </c>
@@ -1894,7 +1896,7 @@
         <v>44223</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>77</v>
       </c>
@@ -1941,7 +1943,7 @@
         <v>44231</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>86</v>
       </c>
@@ -1988,7 +1990,7 @@
         <v>44231</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>88</v>
       </c>
@@ -2035,7 +2037,7 @@
         <v>44231</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>90</v>
       </c>
@@ -2085,7 +2087,7 @@
         <v>44234</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>98</v>
       </c>
@@ -2135,7 +2137,7 @@
         <v>44234</v>
       </c>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>99</v>
       </c>
@@ -2185,7 +2187,7 @@
         <v>44234</v>
       </c>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>101</v>
       </c>
@@ -2235,7 +2237,7 @@
         <v>44297</v>
       </c>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>108</v>
       </c>
@@ -2285,7 +2287,7 @@
         <v>44297</v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>109</v>
       </c>
@@ -2335,7 +2337,7 @@
         <v>44297</v>
       </c>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>110</v>
       </c>
@@ -2385,7 +2387,7 @@
         <v>44297</v>
       </c>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>111</v>
       </c>
@@ -2435,7 +2437,7 @@
         <v>44258</v>
       </c>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>118</v>
       </c>
@@ -2485,7 +2487,7 @@
         <v>44258</v>
       </c>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>120</v>
       </c>
@@ -2535,7 +2537,7 @@
         <v>44258</v>
       </c>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>121</v>
       </c>

</xml_diff>